<commit_message>
SiteStructure Basic framework added
</commit_message>
<xml_diff>
--- a/SiteStructure.xlsx
+++ b/SiteStructure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,9 +15,59 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>Sub menu</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Wall (Home)</t>
+  </si>
+  <si>
+    <t>About Us</t>
+  </si>
+  <si>
+    <t>Sitemap</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>This page will be similar to FB. It will display he recent advts posted by members. Also it will display the basic bio n img of the user. It will allow creating the advts and posting comments, like etc.           *note: the page will ressemble FB wall bcoz we r going to provide a fb app also and ppl are accostomed to fb... avoiding confusion.</t>
+  </si>
+  <si>
+    <t>This page will provide facilities to search and sort the various offers from users according to budget, location, term, deposit etc and also mark the favorite offers and comment on them.</t>
+  </si>
+  <si>
+    <t>This page will consist of the basic bio of user and his/her profile pic</t>
+  </si>
+  <si>
+    <t>help will be provided consisting of the steps form(creation,deletion,updation) of profile, (creation, updation, deletion) of an advt,etc</t>
+  </si>
+  <si>
+    <t>***v v very imp: Please create ur branch(if not created already), checkout the same and then update the following document.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,16 +75,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -42,18 +138,148 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,36 +569,115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="74.28515625" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
about us added to SiteStructure
</commit_message>
<xml_diff>
--- a/SiteStructure.xlsx
+++ b/SiteStructure.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Menu</t>
   </si>
@@ -54,13 +54,16 @@
     <t>This page will provide facilities to search and sort the various offers from users according to budget, location, term, deposit etc and also mark the favorite offers and comment on them.</t>
   </si>
   <si>
-    <t>This page will consist of the basic bio of user and his/her profile pic</t>
-  </si>
-  <si>
     <t>help will be provided consisting of the steps form(creation,deletion,updation) of profile, (creation, updation, deletion) of an advt,etc</t>
   </si>
   <si>
     <t>***v v very imp: Please create ur branch(if not created already), checkout the same and then update the following document.</t>
+  </si>
+  <si>
+    <t>this page will explain the motive of this website.</t>
+  </si>
+  <si>
+    <t>This page will consist of the basic bio of user and his/her profile pic.</t>
   </si>
 </sst>
 </file>
@@ -250,9 +253,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -264,6 +264,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,7 +576,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -585,34 +588,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
+      <c r="A1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -624,18 +627,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D6" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -647,7 +653,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
about us added by nikhil
</commit_message>
<xml_diff>
--- a/SiteStructure.xlsx
+++ b/SiteStructure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Menu</t>
   </si>
@@ -61,13 +61,16 @@
   </si>
   <si>
     <t>***v v very imp: Please create ur branch(if not created already), checkout the same and then update the following document.</t>
+  </si>
+  <si>
+    <t>will show the information about the site</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,9 +253,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -264,6 +264,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,7 +361,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -393,7 +395,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -569,14 +570,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="18.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" style="4" customWidth="1"/>
@@ -584,39 +585,39 @@
     <col min="4" max="4" width="74.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:4" ht="84" customHeight="1">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="45">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -624,7 +625,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -632,17 +633,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="30">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -660,24 +664,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>